<commit_message>
Work in progress. Modified to make it so calling app calls its created class
</commit_message>
<xml_diff>
--- a/resources/Book1.xlsx
+++ b/resources/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
   <si>
     <t>a little</t>
   </si>
@@ -127,9 +127,6 @@
     <t>tag</t>
   </si>
   <si>
-    <t>word type</t>
-  </si>
-  <si>
     <t>arabic</t>
   </si>
   <si>
@@ -142,15 +139,9 @@
     <t>singular</t>
   </si>
   <si>
-    <t>plural</t>
-  </si>
-  <si>
     <t>ktir</t>
   </si>
   <si>
-    <t>ktar</t>
-  </si>
-  <si>
     <t>3an</t>
   </si>
   <si>
@@ -323,6 +314,9 @@
   </si>
   <si>
     <t>ahle</t>
+  </si>
+  <si>
+    <t>word_type</t>
   </si>
 </sst>
 </file>
@@ -678,7 +672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,20 +690,18 @@
         <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
@@ -725,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -743,11 +735,9 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
@@ -763,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -781,7 +771,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -799,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -817,7 +807,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -835,7 +825,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -853,7 +843,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -871,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -889,7 +879,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -907,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -925,7 +915,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -943,7 +933,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -961,7 +951,7 @@
         <v>13</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -979,277 +969,277 @@
         <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F29" s="2"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F30" s="2"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F31" s="2"/>
     </row>

</xml_diff>